<commit_message>
modified:   configs/mapeamentos_substituicoes_ate_60.json new file:   exemplos/anun.xlsx new file:   exemplos/anuncios.xlsx modified:   exemplos/input.xlsx modified:   models_api/api_max.py modified:   models_excel/core.py new file:   models_excel/excel_utils.py new file:   models_excel/teste.xlsx new file:   teste.py
</commit_message>
<xml_diff>
--- a/exemplos/input.xlsx
+++ b/exemplos/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joab.alves\Desktop\api_auto_experts\exemplos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50438E7A-F157-4D5F-9DEC-D3A2B5B3E63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5880EE9-9C9F-4C55-A1F8-449979297624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
   <si>
     <t>Cod Produto</t>
   </si>
@@ -368,9 +368,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A2222B5-085D-46BF-95AB-F9F31E8C2CCF}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -387,6 +389,36 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>